<commit_message>
Started first performance tests for Aufgabe 1
</commit_message>
<xml_diff>
--- a/Materialien/Aufgabe01/Laufzeit_Diagramm.xlsx
+++ b/Materialien/Aufgabe01/Laufzeit_Diagramm.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,23 +123,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -302,19 +312,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>112.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>29320.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -402,19 +412,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>110.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28762.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -442,8 +452,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="570348128"/>
-        <c:axId val="570353224"/>
+        <c:axId val="217138448"/>
+        <c:axId val="217140016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -540,7 +550,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="570348128"/>
+        <c:axId val="217138448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,8 +576,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Durchschnittliche Laufzeit in Millisekunden</a:t>
+                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:t>Anzahl der Klötze</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -639,7 +649,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570353224"/>
+        <c:crossAx val="217140016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -647,7 +657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="570353224"/>
+        <c:axId val="217140016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,18 +697,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Anzahl</a:t>
+                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:t>Durchschnittliche Laufzeit in Millisekunden</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> der Klötze</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2962962962962963E-2"/>
+              <c:y val="0.18008621359687671"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -759,7 +771,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570348128"/>
+        <c:crossAx val="217138448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1397,15 +1409,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1691,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,284 +1716,375 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5">
+      <c r="B2" s="5"/>
+      <c r="C2" s="2">
         <f>AVERAGE(C15:AR15)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2">
         <f>AVERAGE(C26:V26)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+        <v>20.5</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5">
+      <c r="B3" s="5"/>
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C10" si="0">AVERAGE(C16:AR16)</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
+        <v>22.25</v>
+      </c>
+      <c r="D3" s="2">
         <f>AVERAGE(C27:V27)</f>
-        <v>0</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
+      <c r="B4" s="5"/>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>23.25</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D10" si="1">AVERAGE(C28:V28)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>112.75</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>110.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>29320.75</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>28762.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="5">
-        <f t="shared" ref="D4:D10" si="1">AVERAGE(C28:V28)</f>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
+    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
+    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5">
+    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D10" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>22</v>
+      </c>
+      <c r="F16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
         <v>4</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+        <v>23</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>5</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+        <v>114</v>
+      </c>
+      <c r="D18">
+        <v>113</v>
+      </c>
+      <c r="E18">
+        <v>111</v>
+      </c>
+      <c r="F18">
+        <v>113</v>
+      </c>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+        <v>29141</v>
+      </c>
+      <c r="D19">
+        <v>29274</v>
+      </c>
+      <c r="E19">
+        <v>29613</v>
+      </c>
+      <c r="F19">
+        <v>29255</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
         <v>7</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+    <row r="21" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
         <v>8</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
+    <row r="22" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
         <v>9</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+    <row r="23" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
         <v>10</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-    </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+    <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
         <v>2</v>
       </c>
       <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>21</v>
+      </c>
+      <c r="F27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
         <v>4</v>
       </c>
       <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>22</v>
+      </c>
+      <c r="F28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
         <v>5</v>
       </c>
       <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="7">
+        <v>113</v>
+      </c>
+      <c r="D29">
+        <v>109</v>
+      </c>
+      <c r="E29">
+        <v>111</v>
+      </c>
+      <c r="F29">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
+        <v>28632</v>
+      </c>
+      <c r="D30">
+        <v>28736</v>
+      </c>
+      <c r="E30">
+        <v>28803</v>
+      </c>
+      <c r="F30">
+        <v>28878</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
         <v>7</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
+    <row r="32" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
         <v>8</v>
       </c>
       <c r="C32">
@@ -1989,7 +2092,7 @@
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="7">
+      <c r="B33" s="4">
         <v>9</v>
       </c>
       <c r="C33">
@@ -1997,7 +2100,7 @@
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="7">
+      <c r="B34" s="4">
         <v>10</v>
       </c>
       <c r="C34">

</xml_diff>